<commit_message>
updated for 27 March top level numbers - waiting on case level data
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,42 +402,17 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>In Hospital</t>
+          <t>In Hospital Now</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Total In Hospital</t>
+          <t>Total Been In Hospital</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>In ICU</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Community Transmission</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Total Community Transmission</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Tests</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Total Tests</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Test Count</t>
         </is>
       </c>
     </row>
@@ -715,20 +690,6 @@
       <c r="C26">
         <v>102</v>
       </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
-      <c r="L26">
-        <v>2</v>
-      </c>
-      <c r="N26">
-        <v>7459</v>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>Estimate</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
@@ -752,28 +713,11 @@
       <c r="G27">
         <v>12</v>
       </c>
-      <c r="I27">
+      <c r="H27">
         <v>6</v>
       </c>
       <c r="J27">
         <v>0</v>
-      </c>
-      <c r="K27">
-        <v>2</v>
-      </c>
-      <c r="L27">
-        <v>4</v>
-      </c>
-      <c r="M27">
-        <v>900</v>
-      </c>
-      <c r="N27">
-        <v>8359</v>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>Estimate</t>
-        </is>
       </c>
     </row>
     <row r="28">
@@ -798,28 +742,11 @@
       <c r="G28">
         <v>22</v>
       </c>
-      <c r="I28">
+      <c r="H28">
         <v>6</v>
       </c>
       <c r="J28">
         <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>4</v>
-      </c>
-      <c r="M28">
-        <v>1421</v>
-      </c>
-      <c r="N28">
-        <v>9780</v>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>Accurate</t>
-        </is>
       </c>
     </row>
     <row r="29">
@@ -845,30 +772,42 @@
         <v>27</v>
       </c>
       <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29">
         <v>7</v>
       </c>
       <c r="J29">
         <v>0</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>4</v>
-      </c>
-      <c r="M29">
-        <v>2417</v>
-      </c>
-      <c r="N29">
-        <v>12683</v>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>Accurate</t>
-        </is>
+    </row>
+    <row r="30">
+      <c r="A30" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B30">
+        <v>76</v>
+      </c>
+      <c r="C30">
+        <v>338</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>37</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>20</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using the new MoH spreadsheets - not documenting properly until I see how they change ...
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -367,52 +367,62 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>confirmed</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total Confirmed</t>
+          <t>total_confirmed</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Probable</t>
+          <t>probable</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total Probable</t>
+          <t>total_probable</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recovered</t>
+          <t>total</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Total Recovered</t>
+          <t>cumulative_total</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>In Hospital Now</t>
+          <t>recovered</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Total Been In Hospital</t>
+          <t>total_recovered</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>In ICU</t>
+          <t>in_hospital_now</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>total_been_in_hospital</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>in_icu</t>
         </is>
       </c>
     </row>
@@ -426,6 +436,12 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -437,6 +453,12 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -448,6 +470,12 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -459,6 +487,12 @@
       <c r="C5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -470,6 +504,12 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -481,6 +521,12 @@
       <c r="C7">
         <v>2</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
@@ -492,6 +538,12 @@
       <c r="C8">
         <v>3</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -503,6 +555,12 @@
       <c r="C9">
         <v>4</v>
       </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -514,6 +572,12 @@
       <c r="C10">
         <v>5</v>
       </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -525,6 +589,12 @@
       <c r="C11">
         <v>5</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -536,6 +606,12 @@
       <c r="C12">
         <v>5</v>
       </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -547,6 +623,12 @@
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -558,6 +640,12 @@
       <c r="C14">
         <v>5</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
@@ -569,6 +657,12 @@
       <c r="C15">
         <v>5</v>
       </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -580,6 +674,12 @@
       <c r="C16">
         <v>5</v>
       </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -591,6 +691,12 @@
       <c r="C17">
         <v>6</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -602,6 +708,12 @@
       <c r="C18">
         <v>8</v>
       </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>18</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -613,6 +725,12 @@
       <c r="C19">
         <v>8</v>
       </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -624,6 +742,12 @@
       <c r="C20">
         <v>12</v>
       </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>24</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -635,6 +759,12 @@
       <c r="C21">
         <v>20</v>
       </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>32</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -646,6 +776,12 @@
       <c r="C22">
         <v>28</v>
       </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>40</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -657,6 +793,12 @@
       <c r="C23">
         <v>39</v>
       </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+      <c r="G23">
+        <v>51</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
@@ -668,6 +810,12 @@
       <c r="C24">
         <v>52</v>
       </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>64</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
@@ -679,6 +827,12 @@
       <c r="C25">
         <v>66</v>
       </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>78</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
@@ -690,6 +844,12 @@
       <c r="C26">
         <v>102</v>
       </c>
+      <c r="F26">
+        <v>36</v>
+      </c>
+      <c r="G26">
+        <v>114</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
@@ -708,15 +868,21 @@
         <v>13</v>
       </c>
       <c r="F27">
+        <v>53</v>
+      </c>
+      <c r="G27">
+        <v>167</v>
+      </c>
+      <c r="H27">
         <v>12</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>12</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>6</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>0</v>
       </c>
     </row>
@@ -737,15 +903,21 @@
         <v>16</v>
       </c>
       <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>217</v>
+      </c>
+      <c r="H28">
         <v>10</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>22</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>6</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>0</v>
       </c>
     </row>
@@ -766,15 +938,21 @@
         <v>21</v>
       </c>
       <c r="F29">
+        <v>78</v>
+      </c>
+      <c r="G29">
+        <v>295</v>
+      </c>
+      <c r="H29">
         <v>5</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>27</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>7</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>0</v>
       </c>
     </row>
@@ -795,19 +973,63 @@
         <v>30</v>
       </c>
       <c r="F30">
+        <v>85</v>
+      </c>
+      <c r="G30">
+        <v>380</v>
+      </c>
+      <c r="H30">
         <v>10</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>37</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>8</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>20</v>
       </c>
-      <c r="J30">
-        <v>1</v>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B31">
+        <v>78</v>
+      </c>
+      <c r="C31">
+        <v>416</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>35</v>
+      </c>
+      <c r="F31">
+        <v>83</v>
+      </c>
+      <c r="G31">
+        <v>463</v>
+      </c>
+      <c r="H31">
+        <v>13</v>
+      </c>
+      <c r="I31">
+        <v>50</v>
+      </c>
+      <c r="J31">
+        <v>12</v>
+      </c>
+      <c r="K31">
+        <v>22</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st of April update
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1162,6 +1162,106 @@
         <v>9</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" s="2">
+        <v>43921</v>
+      </c>
+      <c r="B34">
+        <v>48</v>
+      </c>
+      <c r="C34">
+        <v>600</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>47</v>
+      </c>
+      <c r="F34">
+        <v>58</v>
+      </c>
+      <c r="G34">
+        <v>647</v>
+      </c>
+      <c r="H34">
+        <v>11</v>
+      </c>
+      <c r="I34">
+        <v>74</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="K34">
+        <v>30</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>343</v>
+      </c>
+      <c r="P34">
+        <v>188</v>
+      </c>
+      <c r="Q34">
+        <v>110</v>
+      </c>
+      <c r="R34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B35">
+        <v>47</v>
+      </c>
+      <c r="C35">
+        <v>647</v>
+      </c>
+      <c r="D35">
+        <v>14</v>
+      </c>
+      <c r="E35">
+        <v>61</v>
+      </c>
+      <c r="F35">
+        <v>61</v>
+      </c>
+      <c r="G35">
+        <v>708</v>
+      </c>
+      <c r="H35">
+        <v>8</v>
+      </c>
+      <c r="I35">
+        <v>82</v>
+      </c>
+      <c r="J35">
+        <v>16</v>
+      </c>
+      <c r="K35">
+        <v>32</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dealing with "Unknown" being added to Ministry spreadsheet - not a bool anymore
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,12 +447,17 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>overseasAndContact</t>
+          <t>investigating</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
           <t>community</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>established</t>
         </is>
       </c>
     </row>
@@ -1149,17 +1154,173 @@
       <c r="N33">
         <v>1</v>
       </c>
-      <c r="O33">
-        <v>259</v>
-      </c>
-      <c r="P33">
-        <v>118</v>
-      </c>
-      <c r="Q33">
-        <v>68</v>
-      </c>
-      <c r="R33">
+    </row>
+    <row r="34">
+      <c r="A34" s="2">
+        <v>43921</v>
+      </c>
+      <c r="B34">
+        <v>48</v>
+      </c>
+      <c r="C34">
+        <v>600</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>47</v>
+      </c>
+      <c r="F34">
+        <v>58</v>
+      </c>
+      <c r="G34">
+        <v>647</v>
+      </c>
+      <c r="H34">
+        <v>11</v>
+      </c>
+      <c r="I34">
+        <v>74</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>343</v>
+      </c>
+      <c r="P34">
+        <v>188</v>
+      </c>
+      <c r="Q34">
+        <v>110</v>
+      </c>
+      <c r="R34">
+        <v>6</v>
+      </c>
+      <c r="S34">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B35">
+        <v>47</v>
+      </c>
+      <c r="C35">
+        <v>647</v>
+      </c>
+      <c r="D35">
+        <v>14</v>
+      </c>
+      <c r="E35">
+        <v>61</v>
+      </c>
+      <c r="F35">
+        <v>61</v>
+      </c>
+      <c r="G35">
+        <v>708</v>
+      </c>
+      <c r="H35">
         <v>9</v>
+      </c>
+      <c r="I35">
+        <v>83</v>
+      </c>
+      <c r="J35">
+        <v>14</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>361</v>
+      </c>
+      <c r="P35">
+        <v>212</v>
+      </c>
+      <c r="Q35">
+        <v>127</v>
+      </c>
+      <c r="R35">
+        <v>7</v>
+      </c>
+      <c r="S35">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B36">
+        <v>76</v>
+      </c>
+      <c r="C36">
+        <v>723</v>
+      </c>
+      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>74</v>
+      </c>
+      <c r="F36">
+        <v>89</v>
+      </c>
+      <c r="G36">
+        <v>797</v>
+      </c>
+      <c r="H36">
+        <v>9</v>
+      </c>
+      <c r="I36">
+        <v>92</v>
+      </c>
+      <c r="J36">
+        <v>13</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>406</v>
+      </c>
+      <c r="P36">
+        <v>247</v>
+      </c>
+      <c r="Q36">
+        <v>135</v>
+      </c>
+      <c r="R36">
+        <v>8</v>
+      </c>
+      <c r="S36">
+        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using esr data to fill in missing MoH data
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1323,6 +1323,62 @@
         <v>797</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B37">
+        <v>49</v>
+      </c>
+      <c r="C37">
+        <v>772</v>
+      </c>
+      <c r="D37">
+        <v>22</v>
+      </c>
+      <c r="E37">
+        <v>96</v>
+      </c>
+      <c r="F37">
+        <v>71</v>
+      </c>
+      <c r="G37">
+        <v>868</v>
+      </c>
+      <c r="H37">
+        <v>11</v>
+      </c>
+      <c r="I37">
+        <v>103</v>
+      </c>
+      <c r="J37">
+        <v>13</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>425</v>
+      </c>
+      <c r="P37">
+        <v>286</v>
+      </c>
+      <c r="Q37">
+        <v>148</v>
+      </c>
+      <c r="R37">
+        <v>9</v>
+      </c>
+      <c r="S37">
+        <v>868</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
manual update from press conference
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1648,10 +1648,10 @@
         <v>1039</v>
       </c>
       <c r="H39">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="I39">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="J39">
         <v>15</v>
@@ -1681,6 +1681,67 @@
         <v>1039</v>
       </c>
       <c r="T39" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>911</v>
+      </c>
+      <c r="D40">
+        <v>28</v>
+      </c>
+      <c r="E40">
+        <v>195</v>
+      </c>
+      <c r="F40">
+        <v>67</v>
+      </c>
+      <c r="G40">
+        <v>1106</v>
+      </c>
+      <c r="H40">
+        <v>20</v>
+      </c>
+      <c r="I40">
+        <v>176</v>
+      </c>
+      <c r="J40">
+        <v>13</v>
+      </c>
+      <c r="L40">
+        <v>3</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>476</v>
+      </c>
+      <c r="P40">
+        <v>420</v>
+      </c>
+      <c r="Q40">
+        <v>188</v>
+      </c>
+      <c r="R40">
+        <v>22</v>
+      </c>
+      <c r="S40">
+        <v>1106</v>
+      </c>
+      <c r="T40" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>

</xml_diff>

<commit_message>
9 April - backfill from ESR
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1808,6 +1808,128 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B42">
+        <v>26</v>
+      </c>
+      <c r="C42">
+        <v>969</v>
+      </c>
+      <c r="D42">
+        <v>24</v>
+      </c>
+      <c r="E42">
+        <v>241</v>
+      </c>
+      <c r="F42">
+        <v>50</v>
+      </c>
+      <c r="G42">
+        <v>1210</v>
+      </c>
+      <c r="H42">
+        <v>41</v>
+      </c>
+      <c r="I42">
+        <v>282</v>
+      </c>
+      <c r="J42">
+        <v>12</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>496</v>
+      </c>
+      <c r="P42">
+        <v>520</v>
+      </c>
+      <c r="Q42">
+        <v>169</v>
+      </c>
+      <c r="R42">
+        <v>24</v>
+      </c>
+      <c r="S42">
+        <v>1210</v>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B43">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>992</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>247</v>
+      </c>
+      <c r="F43">
+        <v>29</v>
+      </c>
+      <c r="G43">
+        <v>1239</v>
+      </c>
+      <c r="H43">
+        <v>35</v>
+      </c>
+      <c r="I43">
+        <v>317</v>
+      </c>
+      <c r="J43">
+        <v>14</v>
+      </c>
+      <c r="L43">
+        <v>4</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>508</v>
+      </c>
+      <c r="P43">
+        <v>545</v>
+      </c>
+      <c r="Q43">
+        <v>161</v>
+      </c>
+      <c r="R43">
+        <v>25</v>
+      </c>
+      <c r="S43">
+        <v>1239</v>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
April 14th - include approximate mapping from reported to announced date
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1930,6 +1930,311 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B44">
+        <v>23</v>
+      </c>
+      <c r="C44">
+        <v>1015</v>
+      </c>
+      <c r="D44">
+        <v>21</v>
+      </c>
+      <c r="E44">
+        <v>268</v>
+      </c>
+      <c r="F44">
+        <v>44</v>
+      </c>
+      <c r="G44">
+        <v>1283</v>
+      </c>
+      <c r="H44">
+        <v>56</v>
+      </c>
+      <c r="I44">
+        <v>373</v>
+      </c>
+      <c r="J44">
+        <v>16</v>
+      </c>
+      <c r="L44">
+        <v>4</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>2</v>
+      </c>
+      <c r="O44">
+        <v>513</v>
+      </c>
+      <c r="P44">
+        <v>565</v>
+      </c>
+      <c r="Q44">
+        <v>180</v>
+      </c>
+      <c r="R44">
+        <v>26</v>
+      </c>
+      <c r="S44">
+        <v>1283</v>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>1035</v>
+      </c>
+      <c r="D45">
+        <v>9</v>
+      </c>
+      <c r="E45">
+        <v>277</v>
+      </c>
+      <c r="F45">
+        <v>29</v>
+      </c>
+      <c r="G45">
+        <v>1312</v>
+      </c>
+      <c r="H45">
+        <v>49</v>
+      </c>
+      <c r="I45">
+        <v>422</v>
+      </c>
+      <c r="J45">
+        <v>15</v>
+      </c>
+      <c r="L45">
+        <v>5</v>
+      </c>
+      <c r="M45">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+      <c r="O45">
+        <v>525</v>
+      </c>
+      <c r="P45">
+        <v>604</v>
+      </c>
+      <c r="Q45">
+        <v>144</v>
+      </c>
+      <c r="R45">
+        <v>26</v>
+      </c>
+      <c r="S45">
+        <v>1312</v>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B46">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>1049</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>281</v>
+      </c>
+      <c r="F46">
+        <v>18</v>
+      </c>
+      <c r="G46">
+        <v>1330</v>
+      </c>
+      <c r="H46">
+        <v>49</v>
+      </c>
+      <c r="I46">
+        <v>471</v>
+      </c>
+      <c r="J46">
+        <v>14</v>
+      </c>
+      <c r="L46">
+        <v>5</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>4</v>
+      </c>
+      <c r="O46">
+        <v>532</v>
+      </c>
+      <c r="P46">
+        <v>625</v>
+      </c>
+      <c r="Q46">
+        <v>146</v>
+      </c>
+      <c r="R46">
+        <v>27</v>
+      </c>
+      <c r="S46">
+        <v>1330</v>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="C47">
+        <v>1064</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>285</v>
+      </c>
+      <c r="F47">
+        <v>19</v>
+      </c>
+      <c r="G47">
+        <v>1349</v>
+      </c>
+      <c r="H47">
+        <v>75</v>
+      </c>
+      <c r="I47">
+        <v>546</v>
+      </c>
+      <c r="J47">
+        <v>15</v>
+      </c>
+      <c r="L47">
+        <v>4</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>5</v>
+      </c>
+      <c r="O47">
+        <v>540</v>
+      </c>
+      <c r="P47">
+        <v>634</v>
+      </c>
+      <c r="Q47">
+        <v>148</v>
+      </c>
+      <c r="R47">
+        <v>27</v>
+      </c>
+      <c r="S47">
+        <v>1349</v>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>1072</v>
+      </c>
+      <c r="D48">
+        <v>9</v>
+      </c>
+      <c r="E48">
+        <v>294</v>
+      </c>
+      <c r="F48">
+        <v>17</v>
+      </c>
+      <c r="G48">
+        <v>1366</v>
+      </c>
+      <c r="H48">
+        <v>82</v>
+      </c>
+      <c r="I48">
+        <v>628</v>
+      </c>
+      <c r="J48">
+        <v>15</v>
+      </c>
+      <c r="L48">
+        <v>3</v>
+      </c>
+      <c r="M48">
+        <v>4</v>
+      </c>
+      <c r="N48">
+        <v>9</v>
+      </c>
+      <c r="O48">
+        <v>533</v>
+      </c>
+      <c r="P48">
+        <v>656</v>
+      </c>
+      <c r="Q48">
+        <v>150</v>
+      </c>
+      <c r="R48">
+        <v>27</v>
+      </c>
+      <c r="S48">
+        <v>1366</v>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
work around removal of Uruguay cases
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -2667,10 +2667,10 @@
         <v>43943</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2679,10 +2679,10 @@
         <v>338</v>
       </c>
       <c r="F56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G56">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="H56">
         <v>30</v>
@@ -2731,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -2743,7 +2743,7 @@
         <v>3</v>
       </c>
       <c r="G57">
-        <v>1454</v>
+        <v>1451</v>
       </c>
       <c r="H57">
         <v>29</v>
@@ -2764,10 +2764,10 @@
         <v>16</v>
       </c>
       <c r="O57">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="P57">
-        <v>800</v>
+        <v>813</v>
       </c>
       <c r="Q57">
         <v>29</v>
@@ -2776,7 +2776,7 @@
         <v>58</v>
       </c>
       <c r="S57">
-        <v>1454</v>
+        <v>1451</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>

</xml_diff>